<commit_message>
- Activities change,  - removed Farmer name field  - Added Agronomist field  - Removed city field. - Agronomist referral data added in User section
Bug fix
- Villages query loading on all pages removed. load on demand set and set to load based LGA filter instead of Area filter
</commit_message>
<xml_diff>
--- a/prod/assets/activities_template.xlsx
+++ b/prod/assets/activities_template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Farmer</t>
   </si>
@@ -46,6 +46,12 @@
     <t>City</t>
   </si>
   <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Agronomist</t>
+  </si>
+  <si>
     <t>John James</t>
   </si>
   <si>
@@ -62,6 +68,12 @@
   </si>
   <si>
     <t>Eziama</t>
+  </si>
+  <si>
+    <t>Ukpo</t>
+  </si>
+  <si>
+    <t>Paul walker</t>
   </si>
 </sst>
 </file>
@@ -395,7 +407,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -425,7 +436,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -451,7 +461,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -477,7 +486,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -503,7 +511,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -529,7 +536,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -555,7 +561,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -581,7 +586,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -607,7 +611,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -633,7 +636,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -684,7 +686,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -710,7 +711,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -736,7 +736,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -762,7 +761,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -788,7 +786,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -814,7 +811,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -840,7 +836,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -866,7 +861,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -892,7 +886,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -918,7 +911,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -966,7 +958,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -996,7 +987,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1022,7 +1012,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1048,7 +1037,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1074,7 +1062,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1100,7 +1087,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1126,7 +1112,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1152,7 +1137,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1178,7 +1162,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1204,7 +1187,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1230,7 +1212,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1238,8 +1220,8 @@
   <cols>
     <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="1" customWidth="1"/>
-    <col min="3" max="11" width="8.85156" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="13" width="8.85156" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1276,10 +1258,16 @@
       <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
+      <c r="L1" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>44929</v>
@@ -1289,21 +1277,27 @@
         <v>150</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="2"/>
       <c r="H2" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="L2" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
@@ -1318,6 +1312,8 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" s="5"/>
@@ -1331,6 +1327,8 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="5"/>
@@ -1344,6 +1342,8 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="5"/>
@@ -1357,6 +1357,8 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="5"/>
@@ -1370,6 +1372,8 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="5"/>
@@ -1383,6 +1387,8 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="5"/>
@@ -1396,19 +1402,8 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>